<commit_message>
Display gantt in nw.js
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -509,7 +509,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:ns10="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:ns13="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:ns20="urn:schemas-microsoft-com:office:excel" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:ns22="urn:schemas-microsoft-com:office:powerpoint" xmlns:ns24="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:odx="http://opendope.org/xpaths" xmlns:odc="http://opendope.org/conditions" xmlns:odq="http://opendope.org/questions" xmlns:oda="http://opendope.org/answers" xmlns:odi="http://opendope.org/components" xmlns:odgm="http://opendope.org/SmartArt/DataHierarchy" xmlns:b="http://schemas.openxmlformats.org/officeDocument/2006/bibliography" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:ns34="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:ns35="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas">
+<xdr:wsDr xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:ns10="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:ns13="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:ns20="urn:schemas-microsoft-com:office:excel" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:ns22="urn:schemas-microsoft-com:office:powerpoint" xmlns:ns24="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:odx="http://opendope.org/xpaths" xmlns:odc="http://opendope.org/conditions" xmlns:odq="http://opendope.org/questions" xmlns:oda="http://opendope.org/answers" xmlns:odi="http://opendope.org/components" xmlns:odgm="http://opendope.org/SmartArt/DataHierarchy" xmlns:b="http://schemas.openxmlformats.org/officeDocument/2006/bibliography" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:ns34="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:ns35="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
@@ -558,7 +558,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:ns10="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:ns13="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:ns20="urn:schemas-microsoft-com:office:excel" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:ns22="urn:schemas-microsoft-com:office:powerpoint" xmlns:ns24="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:odx="http://opendope.org/xpaths" xmlns:odc="http://opendope.org/conditions" xmlns:odq="http://opendope.org/questions" xmlns:oda="http://opendope.org/answers" xmlns:odi="http://opendope.org/components" xmlns:odgm="http://opendope.org/SmartArt/DataHierarchy" xmlns:b="http://schemas.openxmlformats.org/officeDocument/2006/bibliography" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:ns34="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:ns35="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" name="Office 主题">
+<a:theme xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:w15="http://schemas.microsoft.com/office/word/2012/wordml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:ns10="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:ns13="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:ns20="urn:schemas-microsoft-com:office:excel" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:ns22="urn:schemas-microsoft-com:office:powerpoint" xmlns:ns24="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:odx="http://opendope.org/xpaths" xmlns:odc="http://opendope.org/conditions" xmlns:odq="http://opendope.org/questions" xmlns:oda="http://opendope.org/answers" xmlns:odi="http://opendope.org/components" xmlns:odgm="http://opendope.org/SmartArt/DataHierarchy" xmlns:b="http://schemas.openxmlformats.org/officeDocument/2006/bibliography" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:ns34="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:ns35="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1037,7 +1037,9 @@
       <c r="B5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="24"/>
+      <c r="C5" s="25" t="n">
+        <v>1.0</v>
+      </c>
       <c r="D5" s="24"/>
       <c r="E5" s="27"/>
       <c r="F5" s="27"/>

</xml_diff>